<commit_message>
Season1 Resign Contract Fix
</commit_message>
<xml_diff>
--- a/Files/Madden24/IE/Test/Expected Salary.xlsx
+++ b/Files/Madden24/IE/Test/Expected Salary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40f61192ff96ff75/Documents/Git/maddenstats/Files/Madden24/IE/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5873" documentId="13_ncr:1_{ADED6FFD-BF9D-425E-B0E9-69FF67D7C25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{563B6575-C4B8-4297-9DCA-489F565E4B73}"/>
+  <xr:revisionPtr revIDLastSave="5879" documentId="13_ncr:1_{ADED6FFD-BF9D-425E-B0E9-69FF67D7C25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B40BD4F5-1327-468E-8E10-D01A20DC2301}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="24" r:id="rId1"/>
@@ -160,10 +160,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -490,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6200DA08-E509-45AF-AE2B-CB0FB74399A3}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -546,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C4">
         <v>76</v>
@@ -563,7 +559,7 @@
         <v>67</v>
       </c>
       <c r="C5">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1652,7 +1648,7 @@
         <v>16</v>
       </c>
       <c r="B83" s="1">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C83">
         <v>79</v>
@@ -1669,7 +1665,7 @@
         <v>1</v>
       </c>
       <c r="C84">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -1708,7 +1704,7 @@
         <v>17</v>
       </c>
       <c r="B87" s="1">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C87">
         <v>79</v>
@@ -1725,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="C88">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D88">
         <v>1</v>

</xml_diff>